<commit_message>
TMS TT stimuli generation
</commit_message>
<xml_diff>
--- a/Verhalen_Emotional+Arousal_ValidResponses.xlsx
+++ b/Verhalen_Emotional+Arousal_ValidResponses.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuchaowang/Documents/GitHub/RStudio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F7662B-68F4-524B-924F-5EC43D2E83BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB6907B-7728-DC49-A0A4-F5D15CA39A37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="460" windowWidth="27580" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3300" uniqueCount="2071">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3296" uniqueCount="2067">
   <si>
     <t>StartDate</t>
   </si>
@@ -6287,18 +6290,6 @@
   </si>
   <si>
     <t>4: eng,5: wijf,,13: flat,14: alleen,24: Ze,25: praat,26: tegen,27: niemand.`,28: `Ze,29: woont,30: hier,31: helemaal,32: alleen,33: met,34: haar,35: siamese,36: kater`,,48: Mijn,49: scherpe,50: vingernagels,51: schrammen,52: mijn,53: knie√´n.,58: kruip,59: ik,60: onhoorbaar,61: naar,64: Ondertussen,65: weet,66: ik,67: hoe,68: dat,69: moet.,80: Waarom,81: wilde,82: het,83: beest,84: dit,85: kussen,86: niet,87: met,88: me,89: delen?,95: eruit,96: gooien,97: om,98: deze,99: slaapplek,100: te,101: behouden,102: in,103: mijn,104: eigen,105: flat?</t>
-  </si>
-  <si>
-    <t>MIN</t>
-  </si>
-  <si>
-    <t>MAX</t>
-  </si>
-  <si>
-    <t>AVERAGE</t>
-  </si>
-  <si>
-    <t>STDEV</t>
   </si>
 </sst>
 </file>
@@ -7143,10 +7134,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:OE34"/>
+  <dimension ref="A1:OE29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="NN2" workbookViewId="0">
-      <selection activeCell="NZ35" sqref="NZ35"/>
+      <selection activeCell="NY35" sqref="NY31:NZ35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -35241,42 +35232,6 @@
         <v>95264857</v>
       </c>
     </row>
-    <row r="31" spans="1:395" x14ac:dyDescent="0.2">
-      <c r="NY31" t="s">
-        <v>2067</v>
-      </c>
-      <c r="NZ31">
-        <f>MIN(NZ3:NZ29)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="32" spans="1:395" x14ac:dyDescent="0.2">
-      <c r="NY32" t="s">
-        <v>2068</v>
-      </c>
-      <c r="NZ32">
-        <f>MAX(NZ3:NZ29)</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="389:390" x14ac:dyDescent="0.2">
-      <c r="NY33" t="s">
-        <v>2069</v>
-      </c>
-      <c r="NZ33">
-        <f>AVERAGE(NZ3:NZ29)</f>
-        <v>21.444444444444443</v>
-      </c>
-    </row>
-    <row r="34" spans="389:390" x14ac:dyDescent="0.2">
-      <c r="NY34" t="s">
-        <v>2070</v>
-      </c>
-      <c r="NZ34">
-        <f>STDEV(NZ3:NZ29)</f>
-        <v>2.6066974881776694</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>